<commit_message>
Updatet Zeitplan Continued Programming Signed-off-by: Noa <noa@stojanovic.ch>
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DCUNTERRICHT-01\Noa.herzog\Excel\MA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noa\Documents\Schule\MA_NoaHerzog_19Md\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73667383-BD06-4930-92DE-77AAADC5E5EA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="7478" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Woche 10</t>
   </si>
@@ -119,15 +120,6 @@
     <t>Testphase</t>
   </si>
   <si>
-    <t xml:space="preserve">Bugfixes und evtl </t>
-  </si>
-  <si>
-    <t>weitere Tests</t>
-  </si>
-  <si>
-    <t>Fertigstellung der App</t>
-  </si>
-  <si>
     <t>Nebenbei immer an der</t>
   </si>
   <si>
@@ -137,19 +129,19 @@
     <t>weitermachen.</t>
   </si>
   <si>
-    <t>Allgemeiner Zeitpuffer falls verzögerungen oder Probleme auftauchen</t>
-  </si>
-  <si>
     <t>Nach Woche 31 möchte Ich fertig sein mit meiner Arbeit, damit ich noch etwas von den Ferien habe und stressfrei</t>
   </si>
   <si>
     <t>in die Prima starten kann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schriftliche Arbeit </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,19 +209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,18 +226,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -537,19 +515,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -557,12 +535,12 @@
         <v>22</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="I1" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -570,41 +548,41 @@
         <v>23</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="I2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="I3" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -612,10 +590,10 @@
         <v>24</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -623,10 +601,10 @@
         <v>25</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -634,10 +612,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -645,10 +623,10 @@
         <v>27</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -656,106 +634,100 @@
         <v>28</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -766,7 +738,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -780,12 +752,12 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -796,9 +768,9 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>